<commit_message>
Update input for paper (with changes).xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/input for paper (with changes).xlsx
+++ b/migforecasting/clustering/input for paper (with changes).xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
         <v>17275</v>
       </c>
       <c r="B2" s="2">
-        <v>2501.8274772741524</v>
+        <v>3065.78</v>
       </c>
       <c r="C2" s="2">
         <v>21679.803337394831</v>
@@ -529,7 +529,7 @@
         <v>65842</v>
       </c>
       <c r="B3" s="2">
-        <v>11288.278741702596</v>
+        <v>13832.84</v>
       </c>
       <c r="C3" s="2">
         <v>23969.885793246038</v>
@@ -579,7 +579,7 @@
         <v>110482</v>
       </c>
       <c r="B4" s="2">
-        <v>19387.608375048698</v>
+        <v>23757.889999999996</v>
       </c>
       <c r="C4" s="2">
         <v>23374.655086082195</v>
@@ -629,7 +629,7 @@
         <v>18562</v>
       </c>
       <c r="B5" s="2">
-        <v>3828.3971421088322</v>
+        <v>4691.380000000001</v>
       </c>
       <c r="C5" s="2">
         <v>23669.21548370285</v>
@@ -679,7 +679,7 @@
         <v>28673</v>
       </c>
       <c r="B6" s="2">
-        <v>4366.2796858972679</v>
+        <v>5350.51</v>
       </c>
       <c r="C6" s="2">
         <v>20405.00153078483</v>
@@ -729,7 +729,7 @@
         <v>28434</v>
       </c>
       <c r="B7" s="2">
-        <v>5725</v>
+        <v>5839.5</v>
       </c>
       <c r="C7" s="2">
         <v>20773.66617</v>
@@ -779,7 +779,7 @@
         <v>139565</v>
       </c>
       <c r="B8" s="2">
-        <v>24379.999999999993</v>
+        <v>24867.599999999991</v>
       </c>
       <c r="C8" s="2">
         <v>19874.44096</v>
@@ -829,7 +829,7 @@
         <v>19887.999999999989</v>
       </c>
       <c r="B9" s="2">
-        <v>4481.9999999999982</v>
+        <v>4571.6399999999985</v>
       </c>
       <c r="C9" s="2">
         <v>37917.462079999998</v>
@@ -879,7 +879,7 @@
         <v>65776</v>
       </c>
       <c r="B10" s="2">
-        <v>14881</v>
+        <v>15178.62</v>
       </c>
       <c r="C10" s="2">
         <v>35840.741759999997</v>
@@ -929,7 +929,7 @@
         <v>108665</v>
       </c>
       <c r="B11" s="2">
-        <v>17434.000000000004</v>
+        <v>17782.680000000004</v>
       </c>
       <c r="C11" s="2">
         <v>19751.678240000001</v>
@@ -1229,7 +1229,7 @@
         <v>4183.9999999999918</v>
       </c>
       <c r="B17" s="2">
-        <v>788.99999999999841</v>
+        <v>1057.2599999999979</v>
       </c>
       <c r="C17" s="2">
         <v>20226.367727107965</v>
@@ -1279,7 +1279,7 @@
         <v>95828.000000000015</v>
       </c>
       <c r="B18" s="2">
-        <v>13438.999999999998</v>
+        <v>18008.259999999998</v>
       </c>
       <c r="C18" s="2">
         <v>22455.614878771485</v>
@@ -1329,7 +1329,7 @@
         <v>17569.999999999989</v>
       </c>
       <c r="B19" s="2">
-        <v>1887.9999999999989</v>
+        <v>2529.9199999999983</v>
       </c>
       <c r="C19" s="2">
         <v>19492.420354584516</v>
@@ -1379,7 +1379,7 @@
         <v>120926</v>
       </c>
       <c r="B20" s="2">
-        <v>20037.999999999996</v>
+        <v>26850.919999999995</v>
       </c>
       <c r="C20" s="2">
         <v>26679.61717489058</v>
@@ -1429,7 +1429,7 @@
         <v>50473.999999999993</v>
       </c>
       <c r="B21" s="2">
-        <v>8680.9999999999982</v>
+        <v>11632.539999999997</v>
       </c>
       <c r="C21" s="2">
         <v>20574.743082475143</v>
@@ -1479,7 +1479,7 @@
         <v>47578.999999999993</v>
       </c>
       <c r="B22" s="2">
-        <v>11633.999999999998</v>
+        <v>11983.019999999999</v>
       </c>
       <c r="C22" s="2">
         <v>25430.158580461106</v>
@@ -1529,7 +1529,7 @@
         <v>28553</v>
       </c>
       <c r="B23" s="2">
-        <v>6935.9999999999991</v>
+        <v>7144.079999999999</v>
       </c>
       <c r="C23" s="2">
         <v>35250.545648341838</v>
@@ -1579,7 +1579,7 @@
         <v>79746</v>
       </c>
       <c r="B24" s="2">
-        <v>16843</v>
+        <v>17348.29</v>
       </c>
       <c r="C24" s="2">
         <v>36013.090284106096</v>
@@ -1629,7 +1629,7 @@
         <v>57687</v>
       </c>
       <c r="B25" s="2">
-        <v>11292</v>
+        <v>11630.76</v>
       </c>
       <c r="C25" s="2">
         <v>24299.842428383665</v>
@@ -1679,7 +1679,7 @@
         <v>141368</v>
       </c>
       <c r="B26" s="2">
-        <v>33537</v>
+        <v>34543.11</v>
       </c>
       <c r="C26" s="2">
         <v>27642.948561951056</v>
@@ -1729,7 +1729,7 @@
         <v>23671.999999999989</v>
       </c>
       <c r="B27" s="2">
-        <v>2819.9999999999991</v>
+        <v>3158.3999999999987</v>
       </c>
       <c r="C27" s="2">
         <v>17851.005113971656</v>
@@ -1779,7 +1779,7 @@
         <v>116468</v>
       </c>
       <c r="B28" s="2">
-        <v>21239.000000000004</v>
+        <v>23787.680000000004</v>
       </c>
       <c r="C28" s="2">
         <v>24015.332144548502</v>
@@ -1829,7 +1829,7 @@
         <v>64841.999999999993</v>
       </c>
       <c r="B29" s="2">
-        <v>15028.999999999996</v>
+        <v>16832.479999999996</v>
       </c>
       <c r="C29" s="2">
         <v>26319.181705669933</v>
@@ -1879,7 +1879,7 @@
         <v>64100</v>
       </c>
       <c r="B30" s="2">
-        <v>9192</v>
+        <v>10295.040000000001</v>
       </c>
       <c r="C30" s="2">
         <v>21573.720880582281</v>
@@ -1929,7 +1929,7 @@
         <v>105038</v>
       </c>
       <c r="B31" s="2">
-        <v>11442</v>
+        <v>12815.04</v>
       </c>
       <c r="C31" s="2">
         <v>18535.079522489126</v>

</xml_diff>